<commit_message>
Data from database for mail
</commit_message>
<xml_diff>
--- a/TEST.xlsx
+++ b/TEST.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AkshatKhanna\Desktop\Projects\Transport-Mail-Automation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>ZONE</t>
   </si>
@@ -57,9 +62,6 @@
     <t>TO_DATE</t>
   </si>
   <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
     <t>North</t>
   </si>
   <si>
@@ -76,21 +78,6 @@
   </si>
   <si>
     <t>Chitwan</t>
-  </si>
-  <si>
-    <t>sample1@example.com</t>
-  </si>
-  <si>
-    <t>sample2@example.com</t>
-  </si>
-  <si>
-    <t>sample3@example.com</t>
-  </si>
-  <si>
-    <t>sample4@example.com</t>
-  </si>
-  <si>
-    <t>sample5@example.com</t>
   </si>
 </sst>
 </file>
@@ -411,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -422,7 +409,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +426,7 @@
     <col min="10" max="10" width="25.44140625" customWidth="1"/>
     <col min="11" max="11" width="23.5546875" customWidth="1"/>
     <col min="12" max="12" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
+    <col min="13" max="13" width="28.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -479,13 +466,10 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -497,7 +481,7 @@
         <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>6</v>
@@ -520,13 +504,11 @@
       <c r="L2">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -538,7 +520,7 @@
         <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -555,13 +537,11 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -573,7 +553,7 @@
         <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>7</v>
@@ -590,13 +570,11 @@
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -608,7 +586,7 @@
         <v>114</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -625,13 +603,11 @@
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -643,7 +619,7 @@
         <v>115</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -660,19 +636,10 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="M6" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M4" r:id="rId3"/>
-    <hyperlink ref="M5" r:id="rId4"/>
-    <hyperlink ref="M6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>